<commit_message>
Pintado y Bake de terrenos y escenas: Present, NoWater, LittleWater
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="35">
   <si>
     <t>Sistema de dialogos</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Viernes 23</t>
   </si>
   <si>
-    <t>Lunes 26</t>
-  </si>
-  <si>
     <t>Jueves 29</t>
   </si>
   <si>
@@ -122,16 +119,32 @@
     <t>Pending</t>
   </si>
   <si>
-    <t>In Progress</t>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>Martes 27</t>
+  </si>
+  <si>
+    <t>Crear Modelos 3D NPCS</t>
+  </si>
+  <si>
+    <t>MUY Critico</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -158,8 +171,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -450,7 +464,7 @@
     <col min="5" max="5" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>23</v>
       </c>
@@ -464,10 +478,10 @@
         <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -484,10 +498,10 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -504,10 +518,10 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -527,7 +541,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -546,8 +560,9 @@
       <c r="F5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -558,230 +573,244 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
       </c>
       <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="F12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>
       <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="F13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>15</v>
-      </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
         <v>12</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>16</v>
       </c>
-      <c r="F17" t="s">
-        <v>31</v>
+      <c r="F18" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -789,5 +818,6 @@
     <sortCondition ref="D2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>